<commit_message>
Foi implementado o sistema de backup em todas as listas separadas/todas
</commit_message>
<xml_diff>
--- a/storage/lista_calc_Dermo.xlsx
+++ b/storage/lista_calc_Dermo.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,166 +450,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>5000</v>
-      </c>
-      <c r="B2" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C2" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>5000</v>
-      </c>
-      <c r="B3" t="n">
-        <v>6000</v>
-      </c>
-      <c r="C3" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>5000</v>
-      </c>
-      <c r="B4" t="n">
-        <v>6000</v>
-      </c>
-      <c r="C4" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>5000</v>
-      </c>
-      <c r="B5" t="n">
-        <v>6000</v>
-      </c>
-      <c r="C5" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5000</v>
-      </c>
-      <c r="B6" t="n">
-        <v>6000</v>
-      </c>
-      <c r="C6" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>5000</v>
-      </c>
-      <c r="B7" t="n">
-        <v>6000</v>
-      </c>
-      <c r="C7" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>5000</v>
-      </c>
-      <c r="B8" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C8" t="n">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>500</v>
-      </c>
-      <c r="B9" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C9" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>5000</v>
-      </c>
-      <c r="B10" t="n">
-        <v>6000</v>
-      </c>
-      <c r="C10" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>5000</v>
-      </c>
-      <c r="B11" t="n">
-        <v>6000</v>
-      </c>
-      <c r="C11" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>5000</v>
-      </c>
-      <c r="B12" t="n">
-        <v>6000</v>
-      </c>
-      <c r="C12" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>5000</v>
-      </c>
-      <c r="B13" t="n">
-        <v>6000</v>
-      </c>
-      <c r="C13" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>5000</v>
-      </c>
-      <c r="B14" t="n">
-        <v>6000</v>
-      </c>
-      <c r="C14" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>7847.0</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>7417.0</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>